<commit_message>
With proper formated and including header
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/testdata.xlsx
+++ b/src/test/resources/testdata/testdata.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19716" windowHeight="4200"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="4">
   <si>
     <t>username</t>
   </si>
@@ -29,22 +29,10 @@
     <t>password</t>
   </si>
   <si>
-    <t>ideam9363@gmail.com</t>
-  </si>
-  <si>
     <t>ideam363@gmail.com</t>
   </si>
   <si>
     <t>Mandar@9766</t>
-  </si>
-  <si>
-    <t>ideam963@gmail.com</t>
-  </si>
-  <si>
-    <t>andar@#9766</t>
-  </si>
-  <si>
-    <t>Mandar@#9766</t>
   </si>
 </sst>
 </file>
@@ -362,49 +350,110 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A2" sqref="A2:D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.44140625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="20.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>